<commit_message>
Attempt to fix linking'
</commit_message>
<xml_diff>
--- a/Data/data_catalog.xlsx
+++ b/Data/data_catalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Snow/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\wiki_content\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{F39680B3-F173-F646-A890-EFD8AFD1EFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29D3C7E0-E124-4A51-AB6A-A92051C61C57}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9492E7-0352-412B-BEBE-CEA989C74A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="313">
   <si>
     <t>Importance</t>
   </si>
@@ -1038,18 +1038,144 @@
   <si>
     <t>Bloomberg Terminal</t>
   </si>
+  <si>
+    <t>Condominium Unit-level Characteristics</t>
+  </si>
+  <si>
+    <t>Data collected from listings by valuations. Its quality is highly variable and currently only contains three usable columns for the north tri.</t>
+  </si>
+  <si>
+    <t>Residential Valuations</t>
+  </si>
+  <si>
+    <t>There are a number of fields in this data that are unusable. Hopefully the quality of the data will improve as valuations standardizes their processes.</t>
+  </si>
+  <si>
+    <t>Questionable Gargage Units</t>
+  </si>
+  <si>
+    <t>A list of condo parcels identified as non-livable units in iasWorld that valuation analysts feel are actually livable units.</t>
+  </si>
+  <si>
+    <t>This is data that tries to undo overzealous parking space/storage unit identification either by other members of the valuation team, or data department's non-livable unit detection hueristics.</t>
+  </si>
+  <si>
+    <t>Class Dictionary</t>
+  </si>
+  <si>
+    <t>Assessor class codes and descriptions.</t>
+  </si>
+  <si>
+    <t>Class code</t>
+  </si>
+  <si>
+    <t>Class codes and their associated assessment levels and descriptions can change, but rarely do so.</t>
+  </si>
+  <si>
+    <t>Neighborhood Land Rates</t>
+  </si>
+  <si>
+    <t>Land rates ($ per sqft of land) per Assessor neighborhood.</t>
+  </si>
+  <si>
+    <t>Statute dictates that land pricing needs to be consistent within neighborhoods.</t>
+  </si>
+  <si>
+    <t>Site Land Rates</t>
+  </si>
+  <si>
+    <t>Land rates for specific townhouse (295s ) developments</t>
+  </si>
+  <si>
+    <t>Land pricing needs to be consistent within townhome develpoments for uniformity.</t>
+  </si>
+  <si>
+    <t>O'Hare Noise Monitors</t>
+  </si>
+  <si>
+    <t>O'Hare Noise Contours</t>
+  </si>
+  <si>
+    <t>O'Hare 65 DNL boundary.</t>
+  </si>
+  <si>
+    <t>O'Hare noise monitor locations and readings.</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>Ohare Noise Compatability Commission</t>
+  </si>
+  <si>
+    <t>A bespoke, one-off mapping of O'Hare's 65 decibal noise contour.</t>
+  </si>
+  <si>
+    <t>1996-2020</t>
+  </si>
+  <si>
+    <t>Noise Monitor</t>
+  </si>
+  <si>
+    <t>No longer maintained.</t>
+  </si>
+  <si>
+    <t>Midway Noise Monitors</t>
+  </si>
+  <si>
+    <t>Midway noise monitor locations and readings.</t>
+  </si>
+  <si>
+    <t>2008-2021</t>
+  </si>
+  <si>
+    <t>Chicago Department of Aviation</t>
+  </si>
+  <si>
+    <t>May have ended in 2021.</t>
+  </si>
+  <si>
+    <t>Railroads</t>
+  </si>
+  <si>
+    <t>Metra, CTA, and freight railroads</t>
+  </si>
+  <si>
+    <t>Arbitrary section of rail</t>
+  </si>
+  <si>
+    <t>https://hub-cookcountyil.opendata.arcgis.com/datasets/dfa393be3a104c33a2ae95455c916ccd_3/explore?showTable=true</t>
+  </si>
+  <si>
+    <t>https://www.flychicago.com/community/MDWnoise/ANMS/Pages/ANMSreports.aspx</t>
+  </si>
+  <si>
+    <t>https://oharenoise.org/sitemedia/documents/noise_mitigation/noise_monitors/012322/ORD_Monitors_History_FactSheet.pdf</t>
+  </si>
+  <si>
+    <t>Community Area</t>
+  </si>
+  <si>
+    <t>Subdivisions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1121,71 +1247,73 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{A590425C-8270-4CB9-B88A-2A5DF1FD923D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1497,13 +1625,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.7109375" style="1" customWidth="1"/>
@@ -1523,7 +1652,7 @@
     <col min="18" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="33.950000000000003">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1576,7 +1705,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="32.1">
+    <row r="2" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -1630,7 +1759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="32.1">
+    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1684,7 +1813,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="24" customFormat="1" ht="45">
+    <row r="4" spans="1:17" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>17</v>
       </c>
@@ -1734,7 +1863,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="45">
+    <row r="5" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>44</v>
       </c>
@@ -1788,7 +1917,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="24" customFormat="1" ht="48">
+    <row r="6" spans="1:17" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>53</v>
       </c>
@@ -1842,7 +1971,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="24" customFormat="1" ht="32.1">
+    <row r="7" spans="1:17" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>44</v>
       </c>
@@ -1894,7 +2023,7 @@
       </c>
       <c r="Q7" s="26"/>
     </row>
-    <row r="8" spans="1:17" s="24" customFormat="1" ht="48">
+    <row r="8" spans="1:17" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>17</v>
       </c>
@@ -1948,7 +2077,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="32.1">
+    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>44</v>
       </c>
@@ -1999,7 +2128,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="48">
+    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>75</v>
       </c>
@@ -2053,7 +2182,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="75">
+    <row r="11" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>53</v>
       </c>
@@ -2104,7 +2233,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="48">
+    <row r="12" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>75</v>
       </c>
@@ -2158,7 +2287,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="32.1">
+    <row r="13" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
@@ -2209,7 +2338,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="60">
+    <row r="14" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
@@ -2260,7 +2389,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="30">
+    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>44</v>
       </c>
@@ -2311,7 +2440,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="48">
+    <row r="16" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -2362,7 +2491,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="24" customFormat="1">
+    <row r="17" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>75</v>
       </c>
@@ -2416,7 +2545,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="24" customFormat="1">
+    <row r="18" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>75</v>
       </c>
@@ -2468,7 +2597,7 @@
       </c>
       <c r="Q18" s="29"/>
     </row>
-    <row r="19" spans="1:17" s="24" customFormat="1">
+    <row r="19" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>75</v>
       </c>
@@ -2520,7 +2649,7 @@
       </c>
       <c r="Q19" s="29"/>
     </row>
-    <row r="20" spans="1:17" s="24" customFormat="1">
+    <row r="20" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>75</v>
       </c>
@@ -2572,7 +2701,7 @@
       </c>
       <c r="Q20" s="29"/>
     </row>
-    <row r="21" spans="1:17" s="24" customFormat="1">
+    <row r="21" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>75</v>
       </c>
@@ -2624,7 +2753,7 @@
       </c>
       <c r="Q21" s="29"/>
     </row>
-    <row r="22" spans="1:17" ht="48">
+    <row r="22" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>75</v>
       </c>
@@ -2675,7 +2804,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="63.95">
+    <row r="23" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
@@ -2726,7 +2855,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="75">
+    <row r="24" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>53</v>
       </c>
@@ -2777,7 +2906,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="63.95">
+    <row r="25" spans="1:17" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>53</v>
       </c>
@@ -2828,7 +2957,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="45">
+    <row r="26" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>44</v>
       </c>
@@ -2882,7 +3011,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="32.1">
+    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>44</v>
       </c>
@@ -2928,7 +3057,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="48">
+    <row r="28" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>75</v>
       </c>
@@ -2982,7 +3111,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="24" customFormat="1" ht="32.1">
+    <row r="29" spans="1:17" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>75</v>
       </c>
@@ -3036,7 +3165,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="15.95">
+    <row r="30" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>75</v>
       </c>
@@ -3090,7 +3219,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="32.1">
+    <row r="31" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>44</v>
       </c>
@@ -3132,7 +3261,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="24" customFormat="1" ht="32.1">
+    <row r="32" spans="1:17" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>44</v>
       </c>
@@ -3186,7 +3315,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="32.1">
+    <row r="33" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>44</v>
       </c>
@@ -3237,7 +3366,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15.95">
+    <row r="34" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>44</v>
       </c>
@@ -3288,7 +3417,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="48">
+    <row r="35" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>44</v>
       </c>
@@ -3338,7 +3467,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="60">
+    <row r="36" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>75</v>
       </c>
@@ -3392,7 +3521,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="48">
+    <row r="37" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>75</v>
       </c>
@@ -3446,7 +3575,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="48">
+    <row r="38" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>75</v>
       </c>
@@ -3497,7 +3626,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="32.1">
+    <row r="39" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>44</v>
       </c>
@@ -3548,7 +3677,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="48">
+    <row r="40" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>75</v>
       </c>
@@ -3593,7 +3722,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="32.1">
+    <row r="41" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>75</v>
       </c>
@@ -3633,7 +3762,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="32.1">
+    <row r="42" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>75</v>
       </c>
@@ -3673,7 +3802,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="48">
+    <row r="43" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>75</v>
       </c>
@@ -3713,7 +3842,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="32.1">
+    <row r="44" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>17</v>
       </c>
@@ -3764,7 +3893,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="45">
+    <row r="45" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>17</v>
       </c>
@@ -3815,7 +3944,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="48">
+    <row r="46" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>75</v>
       </c>
@@ -3860,7 +3989,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="48">
+    <row r="47" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>75</v>
       </c>
@@ -3911,7 +4040,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="32.1">
+    <row r="48" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>75</v>
       </c>
@@ -3953,7 +4082,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="32.1">
+    <row r="49" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>75</v>
       </c>
@@ -3994,6 +4123,472 @@
       <c r="Q49" s="11" t="s">
         <v>271</v>
       </c>
+    </row>
+    <row r="50" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G50" s="9">
+        <v>100000</v>
+      </c>
+      <c r="H50" s="9">
+        <v>1</v>
+      </c>
+      <c r="I50" s="9">
+        <v>100000</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N50" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O50" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q50" s="11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G51" s="1">
+        <v>100</v>
+      </c>
+      <c r="H51" s="1">
+        <v>1</v>
+      </c>
+      <c r="I51" s="1">
+        <v>100</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O51" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q51" s="11" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="G52" s="1">
+        <v>200</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+      <c r="I52" s="1">
+        <v>200</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q52" s="11" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G53" s="1">
+        <v>275</v>
+      </c>
+      <c r="H53" s="1">
+        <v>2</v>
+      </c>
+      <c r="I53" s="1">
+        <v>550</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M53" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N53" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O53" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q53" s="11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="G54" s="1">
+        <v>30000</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1</v>
+      </c>
+      <c r="I54" s="1">
+        <v>30000</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O54" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q54" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="G55" s="1">
+        <v>36</v>
+      </c>
+      <c r="H55" s="1">
+        <v>25</v>
+      </c>
+      <c r="I55" s="1">
+        <v>900</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M55" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N55" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="P55" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q55" s="11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E56" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1</v>
+      </c>
+      <c r="H56" s="1">
+        <v>1</v>
+      </c>
+      <c r="I56" s="1">
+        <v>1</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="M56" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N56" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O56" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q56" s="11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="E57" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="G57" s="1">
+        <v>13</v>
+      </c>
+      <c r="H57" s="1">
+        <v>15</v>
+      </c>
+      <c r="I57" s="1">
+        <v>195</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L57" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M57" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N57" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O57" t="s">
+        <v>303</v>
+      </c>
+      <c r="P57" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q57" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="D58" s="16">
+        <v>2021</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="G58" s="1">
+        <v>37000</v>
+      </c>
+      <c r="H58" s="1">
+        <v>1</v>
+      </c>
+      <c r="I58" s="1">
+        <v>37000</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L58" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N58" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O58" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="P58" s="18" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C59"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C60"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="C61"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q49" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -4024,20 +4619,19 @@
     <hyperlink ref="P40" r:id="rId21" xr:uid="{E1F803F9-C747-BC43-AAD3-0A5E3AE077E8}"/>
     <hyperlink ref="P46" r:id="rId22" xr:uid="{20D243A5-1A32-4848-A70A-6E228D4F9C87}"/>
     <hyperlink ref="P12" r:id="rId23" xr:uid="{F0FC8E30-A57F-8B4D-93C3-7D5ABFB17D16}"/>
+    <hyperlink ref="P58" r:id="rId24" xr:uid="{177003CB-AD1A-4440-973C-ACF31D15A861}"/>
+    <hyperlink ref="P55" r:id="rId25" xr:uid="{37132F29-8703-4C40-8B05-4A1CED7BF052}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
-  <legacyDrawing r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
+  <legacyDrawing r:id="rId27"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4232,19 +4826,46 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC6C0C23-8FF2-44C5-9EAA-6C41E24E5BCF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DE10C22-4475-444D-A043-27EEC84CDC3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35C5F5EB-7EE3-4AB6-894B-E52817746A4B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35C5F5EB-7EE3-4AB6-894B-E52817746A4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
+    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DE10C22-4475-444D-A043-27EEC84CDC3B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC6C0C23-8FF2-44C5-9EAA-6C41E24E5BCF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>